<commit_message>
add excel multiple keys support
</commit_message>
<xml_diff>
--- a/Unity/Assets/Config/Excel/SkillLevelConfig.xlsx
+++ b/Unity/Assets/Config/Excel/SkillLevelConfig.xlsx
@@ -5,22 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Nova\Legends-Of-Heroes\Unity\Assets\Config\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sky\Legends-Of-Heroes\Unity\Assets\Config\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09358D06-89B1-4E0C-926D-417B0173FDC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE1C20FC-899F-4500-8D41-DE2836D382F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22410" yWindow="1200" windowWidth="22800" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SkillLevel" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t>#</t>
   </si>
@@ -58,7 +58,19 @@
     <t>强力攻击技能</t>
   </si>
   <si>
-    <t>扩散吞噬</t>
+    <t>key</t>
+  </si>
+  <si>
+    <t>扩散吞噬1级</t>
+  </si>
+  <si>
+    <t>扩散吞噬2级</t>
+  </si>
+  <si>
+    <t>扩散吞噬3级</t>
+  </si>
+  <si>
+    <t>扩散吞噬4级</t>
   </si>
 </sst>
 </file>
@@ -430,7 +442,7 @@
   <dimension ref="C2:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -439,12 +451,18 @@
     <col min="2" max="2" width="12.7109375" style="2" customWidth="1"/>
     <col min="3" max="4" width="12.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="15.140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.7109375" style="2" customWidth="1"/>
     <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:7">
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
@@ -510,20 +528,62 @@
         <v>3</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="3:7" s="1" customFormat="1">
-      <c r="G7" s="4"/>
+      <c r="C7" s="1">
+        <v>1001</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="3:7" s="1" customFormat="1">
-      <c r="G8" s="4"/>
+      <c r="C8" s="1">
+        <v>1001</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" spans="3:7" s="1" customFormat="1">
-      <c r="G9" s="4"/>
+      <c r="C9" s="1">
+        <v>1001</v>
+      </c>
+      <c r="D9" s="1">
+        <v>4</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>